<commit_message>
Chicago zip codes and ranked heatmap
</commit_message>
<xml_diff>
--- a/SiteBackend/static/Zips Retrieved.xlsx
+++ b/SiteBackend/static/Zips Retrieved.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josh/Documents/GitHub/GroupProject/CSE6242GroupProject/SiteBackend/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D139ED3-0379-3241-B1DB-8C9900A159C1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419746EA-7422-4D47-9CBB-2331076C68A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{19429350-E7BE-2742-A483-7B39BDF6B205}"/>
+    <workbookView xWindow="13440" yWindow="460" windowWidth="18020" windowHeight="20540" xr2:uid="{19429350-E7BE-2742-A483-7B39BDF6B205}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,7 +463,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1375FCE5-0DF9-994C-AB85-C088B0D5B9BA}">
   <dimension ref="A1:E5045"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A5001" workbookViewId="0">
+      <selection activeCell="E5029" sqref="E5029"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -86236,6 +86238,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E5045" xr:uid="{A0C4193E-5EE2-2143-81C6-DF0BF2AC9E0E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>